<commit_message>
Add formatting to worked-examples vignette
</commit_message>
<xml_diff>
--- a/inst/extdata/worked-examples.xlsx
+++ b/inst/extdata/worked-examples.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="13785" windowHeight="12660" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="13785" windowHeight="12660" firstSheet="13" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="clean" sheetId="17" r:id="rId1"/>
@@ -24,13 +24,15 @@
     <sheet name="performance" sheetId="14" r:id="rId15"/>
     <sheet name="female" sheetId="15" r:id="rId16"/>
     <sheet name="male" sheetId="16" r:id="rId17"/>
+    <sheet name="formatting" sheetId="18" r:id="rId18"/>
+    <sheet name="in-cell formatting" sheetId="19" r:id="rId19"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="57">
   <si>
     <t>Title text</t>
   </si>
@@ -156,13 +158,141 @@
   </si>
   <si>
     <t>By subject</t>
+  </si>
+  <si>
+    <t>bold</t>
+  </si>
+  <si>
+    <t>italic</t>
+  </si>
+  <si>
+    <t>underline</t>
+  </si>
+  <si>
+    <t>strikethrough</t>
+  </si>
+  <si>
+    <t>yellow fill</t>
+  </si>
+  <si>
+    <t>red text</t>
+  </si>
+  <si>
+    <t>font size 14</t>
+  </si>
+  <si>
+    <t>font arial</t>
+  </si>
+  <si>
+    <t>black border</t>
+  </si>
+  <si>
+    <t>thick border</t>
+  </si>
+  <si>
+    <t>dashed border</t>
+  </si>
+  <si>
+    <t>row height 30</t>
+  </si>
+  <si>
+    <t>column width 16.76</t>
+  </si>
+  <si>
+    <t>Bad' style</t>
+  </si>
+  <si>
+    <r>
+      <t>in-cell:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bold,</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>italic,</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>underline,</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>strikethrough,</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>superscript,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>red,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>arial,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>size 14</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,6 +456,53 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -520,7 +697,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -789,6 +966,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="mediumDashed">
+        <color indexed="64"/>
+      </left>
+      <right style="mediumDashed">
+        <color indexed="64"/>
+      </right>
+      <top style="mediumDashed">
+        <color indexed="64"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -835,7 +1040,7 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -898,6 +1103,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="7" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1408,15 +1620,15 @@
       </c>
       <c r="D3" s="43">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E3" s="43">
         <f t="shared" ref="E3:F18" ca="1" si="0">RANDBETWEEN(0,9)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -1426,15 +1638,15 @@
       </c>
       <c r="D4" s="43">
         <f t="shared" ref="D4:D6" ca="1" si="1">RANDBETWEEN(0,9)</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E4" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -1444,15 +1656,15 @@
       </c>
       <c r="D5" s="43">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -1462,15 +1674,15 @@
       </c>
       <c r="D6" s="43">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E6" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -1495,15 +1707,15 @@
       </c>
       <c r="D8" s="43">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E8" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -1513,11 +1725,11 @@
       </c>
       <c r="D9" s="43">
         <f t="shared" ref="D9:D11" ca="1" si="2">RANDBETWEEN(0,9)</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E9" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F9" s="28">
         <f t="shared" ca="1" si="0"/>
@@ -1535,11 +1747,11 @@
       </c>
       <c r="E10" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -1553,11 +1765,11 @@
       </c>
       <c r="E11" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F11" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -1582,7 +1794,7 @@
       </c>
       <c r="D13" s="43">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E13" s="43">
         <f t="shared" ca="1" si="0"/>
@@ -1590,7 +1802,7 @@
       </c>
       <c r="F13" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -1600,15 +1812,15 @@
       </c>
       <c r="D14" s="43">
         <f t="shared" ref="D14:D16" ca="1" si="3">RANDBETWEEN(0,9)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E14" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F14" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -1618,11 +1830,11 @@
       </c>
       <c r="D15" s="43">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E15" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F15" s="28">
         <f t="shared" ca="1" si="0"/>
@@ -1636,15 +1848,15 @@
       </c>
       <c r="D16" s="43">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E16" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F16" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -1669,15 +1881,15 @@
       </c>
       <c r="D18" s="43">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E18" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F18" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -1691,11 +1903,11 @@
       </c>
       <c r="E19" s="43">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F19" s="28">
         <f t="shared" ca="1" si="4"/>
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -1705,15 +1917,15 @@
       </c>
       <c r="D20" s="43">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E20" s="43">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F20" s="28">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -1723,15 +1935,15 @@
       </c>
       <c r="D21" s="42">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E21" s="42">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F21" s="30">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1773,15 +1985,15 @@
       </c>
       <c r="C4" s="25">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="D4" s="47">
         <f t="shared" ref="D4:E7" ca="1" si="0">RANDBETWEEN(0,9)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E4" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -1794,11 +2006,11 @@
       </c>
       <c r="D5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -1807,15 +2019,15 @@
       </c>
       <c r="C6" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D6" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
@@ -1824,7 +2036,7 @@
       </c>
       <c r="C7" s="29">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" s="42">
         <f t="shared" ca="1" si="0"/>
@@ -1832,7 +2044,7 @@
       </c>
       <c r="E7" s="30">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
@@ -1861,15 +2073,15 @@
       </c>
       <c r="C10" s="25">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D10" s="47">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E10" s="26">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -1878,15 +2090,15 @@
       </c>
       <c r="C11" s="27">
         <f t="shared" ref="C11:C13" ca="1" si="2">RANDBETWEEN(0,9)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D11" s="43">
         <f t="shared" ref="D11:E13" ca="1" si="3">RANDBETWEEN(0,9)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E11" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
@@ -1895,15 +2107,15 @@
       </c>
       <c r="C12" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D12" s="43">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E12" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -1916,11 +2128,11 @@
       </c>
       <c r="D13" s="42">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E13" s="30">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -1949,15 +2161,15 @@
       </c>
       <c r="C16" s="25">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D16" s="47">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E16" s="26">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -1966,11 +2178,11 @@
       </c>
       <c r="C17" s="27">
         <f t="shared" ref="C17:C19" ca="1" si="4">RANDBETWEEN(0,9)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="43">
         <f t="shared" ref="D17:E19" ca="1" si="5">RANDBETWEEN(0,9)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E17" s="28">
         <f t="shared" ca="1" si="5"/>
@@ -1983,15 +2195,15 @@
       </c>
       <c r="C18" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D18" s="43">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E18" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -2000,15 +2212,15 @@
       </c>
       <c r="C19" s="29">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D19" s="42">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E19" s="30">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -2037,15 +2249,15 @@
       </c>
       <c r="C22" s="25">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D22" s="47">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E22" s="26">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -2054,15 +2266,15 @@
       </c>
       <c r="C23" s="27">
         <f t="shared" ref="C23:E25" ca="1" si="6">RANDBETWEEN(0,9)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D23" s="43">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23" s="28">
         <f t="shared" ca="1" si="6"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -2071,15 +2283,15 @@
       </c>
       <c r="C24" s="27">
         <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="D24" s="43">
         <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E24" s="28">
         <f t="shared" ca="1" si="6"/>
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
@@ -2088,15 +2300,15 @@
       </c>
       <c r="C25" s="29">
         <f t="shared" ca="1" si="6"/>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D25" s="42">
         <f t="shared" ca="1" si="6"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E25" s="30">
         <f t="shared" ca="1" si="6"/>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2458,6 +2670,115 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="52" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="53" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="54" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="55" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="35" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="56" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="57" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="58" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D7"/>
@@ -2734,7 +3055,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>

<commit_message>
Add worked example of in-cell formatting
</commit_message>
<xml_diff>
--- a/inst/extdata/worked-examples.xlsx
+++ b/inst/extdata/worked-examples.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="62">
   <si>
     <t>Title text</t>
   </si>
@@ -287,12 +287,40 @@
       <t>size 14</t>
     </r>
   </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>A1-TEST</t>
+  </si>
+  <si>
+    <t>A3-PRODUCTION</t>
+  </si>
+  <si>
+    <r>
+      <t>A2-</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PRODUCTION</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -502,6 +530,14 @@
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="35">
@@ -1620,15 +1656,15 @@
       </c>
       <c r="D3" s="43">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E3" s="43">
         <f t="shared" ref="E3:F18" ca="1" si="0">RANDBETWEEN(0,9)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -1638,7 +1674,7 @@
       </c>
       <c r="D4" s="43">
         <f t="shared" ref="D4:D6" ca="1" si="1">RANDBETWEEN(0,9)</f>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E4" s="43">
         <f t="shared" ca="1" si="0"/>
@@ -1646,7 +1682,7 @@
       </c>
       <c r="F4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -1660,11 +1696,11 @@
       </c>
       <c r="E5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -1674,15 +1710,15 @@
       </c>
       <c r="D6" s="43">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E6" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -1707,11 +1743,11 @@
       </c>
       <c r="D8" s="43">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E8" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F8" s="28">
         <f t="shared" ca="1" si="0"/>
@@ -1725,15 +1761,15 @@
       </c>
       <c r="D9" s="43">
         <f t="shared" ref="D9:D11" ca="1" si="2">RANDBETWEEN(0,9)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E9" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -1743,7 +1779,7 @@
       </c>
       <c r="D10" s="43">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E10" s="43">
         <f t="shared" ca="1" si="0"/>
@@ -1751,7 +1787,7 @@
       </c>
       <c r="F10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -1761,15 +1797,15 @@
       </c>
       <c r="D11" s="43">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E11" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F11" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -1798,11 +1834,11 @@
       </c>
       <c r="E13" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F13" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -1812,15 +1848,15 @@
       </c>
       <c r="D14" s="43">
         <f t="shared" ref="D14:D16" ca="1" si="3">RANDBETWEEN(0,9)</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E14" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F14" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -1830,15 +1866,15 @@
       </c>
       <c r="D15" s="43">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E15" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F15" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
@@ -1848,15 +1884,15 @@
       </c>
       <c r="D16" s="43">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E16" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F16" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -1885,11 +1921,11 @@
       </c>
       <c r="E18" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F18" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -1899,7 +1935,7 @@
       </c>
       <c r="D19" s="43">
         <f t="shared" ref="D19:F21" ca="1" si="4">RANDBETWEEN(0,9)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E19" s="43">
         <f t="shared" ca="1" si="4"/>
@@ -1907,7 +1943,7 @@
       </c>
       <c r="F19" s="28">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -1921,11 +1957,11 @@
       </c>
       <c r="E20" s="43">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F20" s="28">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -1935,11 +1971,11 @@
       </c>
       <c r="D21" s="42">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E21" s="42">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F21" s="30">
         <f t="shared" ca="1" si="4"/>
@@ -1985,15 +2021,15 @@
       </c>
       <c r="C4" s="25">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D4" s="47">
         <f t="shared" ref="D4:E7" ca="1" si="0">RANDBETWEEN(0,9)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E4" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -2006,11 +2042,11 @@
       </c>
       <c r="D5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -2019,15 +2055,15 @@
       </c>
       <c r="C6" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D6" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
@@ -2036,15 +2072,15 @@
       </c>
       <c r="C7" s="29">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E7" s="30">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
@@ -2073,15 +2109,15 @@
       </c>
       <c r="C10" s="25">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D10" s="47">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" s="26">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -2094,11 +2130,11 @@
       </c>
       <c r="D11" s="43">
         <f t="shared" ref="D11:E13" ca="1" si="3">RANDBETWEEN(0,9)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E11" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
@@ -2107,15 +2143,15 @@
       </c>
       <c r="C12" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D12" s="43">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E12" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -2124,15 +2160,15 @@
       </c>
       <c r="C13" s="29">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D13" s="42">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E13" s="30">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -2165,11 +2201,11 @@
       </c>
       <c r="D16" s="47">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E16" s="26">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -2178,15 +2214,15 @@
       </c>
       <c r="C17" s="27">
         <f t="shared" ref="C17:C19" ca="1" si="4">RANDBETWEEN(0,9)</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D17" s="43">
         <f t="shared" ref="D17:E19" ca="1" si="5">RANDBETWEEN(0,9)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E17" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -2195,7 +2231,7 @@
       </c>
       <c r="C18" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="D18" s="43">
         <f t="shared" ca="1" si="5"/>
@@ -2203,7 +2239,7 @@
       </c>
       <c r="E18" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -2212,15 +2248,15 @@
       </c>
       <c r="C19" s="29">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D19" s="42">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E19" s="30">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -2249,15 +2285,15 @@
       </c>
       <c r="C22" s="25">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D22" s="47">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E22" s="26">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -2266,15 +2302,15 @@
       </c>
       <c r="C23" s="27">
         <f t="shared" ref="C23:E25" ca="1" si="6">RANDBETWEEN(0,9)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D23" s="43">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E23" s="28">
         <f t="shared" ca="1" si="6"/>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -2283,7 +2319,7 @@
       </c>
       <c r="C24" s="27">
         <f t="shared" ca="1" si="6"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D24" s="43">
         <f t="shared" ca="1" si="6"/>
@@ -2300,7 +2336,7 @@
       </c>
       <c r="C25" s="29">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D25" s="42">
         <f t="shared" ca="1" si="6"/>
@@ -2308,7 +2344,7 @@
       </c>
       <c r="E25" s="30">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -2761,17 +2797,52 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add worked-example of superscript symbols
</commit_message>
<xml_diff>
--- a/inst/extdata/worked-examples.xlsx
+++ b/inst/extdata/worked-examples.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="13785" windowHeight="12660" firstSheet="16" activeTab="20"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="13785" windowHeight="12660" firstSheet="12" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="clean" sheetId="17" r:id="rId1"/>
@@ -27,14 +27,15 @@
     <sheet name="male" sheetId="16" r:id="rId18"/>
     <sheet name="formatting" sheetId="18" r:id="rId19"/>
     <sheet name="in-cell formatting" sheetId="19" r:id="rId20"/>
-    <sheet name="non-text headers" sheetId="21" r:id="rId21"/>
+    <sheet name="superscript symbols" sheetId="22" r:id="rId21"/>
+    <sheet name="non-text headers" sheetId="21" r:id="rId22"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="64">
   <si>
     <t>Title text</t>
   </si>
@@ -315,6 +316,38 @@
         <scheme val="minor"/>
       </rPr>
       <t>PRODUCTION</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Paul</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>a</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
     </r>
   </si>
 </sst>
@@ -1078,7 +1111,7 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1131,15 +1164,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1150,6 +1174,17 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="7" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1505,10 +1540,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="48" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1786,15 +1821,15 @@
       </c>
       <c r="D3" s="43">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3" s="43">
         <f t="shared" ref="E3:F18" ca="1" si="0">RANDBETWEEN(0,9)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -1804,15 +1839,15 @@
       </c>
       <c r="D4" s="43">
         <f t="shared" ref="D4:D6" ca="1" si="1">RANDBETWEEN(0,9)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E4" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -1822,15 +1857,15 @@
       </c>
       <c r="D5" s="43">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -1840,7 +1875,7 @@
       </c>
       <c r="D6" s="43">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E6" s="43">
         <f t="shared" ca="1" si="0"/>
@@ -1848,7 +1883,7 @@
       </c>
       <c r="F6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -1873,15 +1908,15 @@
       </c>
       <c r="D8" s="43">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E8" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -1891,15 +1926,15 @@
       </c>
       <c r="D9" s="43">
         <f t="shared" ref="D9:D11" ca="1" si="2">RANDBETWEEN(0,9)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E9" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -1909,15 +1944,15 @@
       </c>
       <c r="D10" s="43">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E10" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -1927,15 +1962,15 @@
       </c>
       <c r="D11" s="43">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E11" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="F11" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -1960,15 +1995,15 @@
       </c>
       <c r="D13" s="43">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E13" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F13" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -1978,15 +2013,15 @@
       </c>
       <c r="D14" s="43">
         <f t="shared" ref="D14:D16" ca="1" si="3">RANDBETWEEN(0,9)</f>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E14" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -1996,15 +2031,15 @@
       </c>
       <c r="D15" s="43">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E15" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="F15" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
@@ -2014,7 +2049,7 @@
       </c>
       <c r="D16" s="43">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E16" s="43">
         <f t="shared" ca="1" si="0"/>
@@ -2022,7 +2057,7 @@
       </c>
       <c r="F16" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -2047,15 +2082,15 @@
       </c>
       <c r="D18" s="43">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E18" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F18" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -2065,15 +2100,15 @@
       </c>
       <c r="D19" s="43">
         <f t="shared" ref="D19:F21" ca="1" si="4">RANDBETWEEN(0,9)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E19" s="43">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F19" s="28">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -2083,7 +2118,7 @@
       </c>
       <c r="D20" s="43">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E20" s="43">
         <f t="shared" ca="1" si="4"/>
@@ -2091,7 +2126,7 @@
       </c>
       <c r="F20" s="28">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -2101,11 +2136,11 @@
       </c>
       <c r="D21" s="42">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E21" s="42">
         <f t="shared" ca="1" si="4"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F21" s="30">
         <f t="shared" ca="1" si="4"/>
@@ -2127,11 +2162,11 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="25"/>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="50"/>
+      <c r="D2" s="59"/>
+      <c r="E2" s="60"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="27"/>
@@ -2151,7 +2186,7 @@
       </c>
       <c r="C4" s="25">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D4" s="47">
         <f t="shared" ref="D4:E7" ca="1" si="0">RANDBETWEEN(0,9)</f>
@@ -2159,7 +2194,7 @@
       </c>
       <c r="E4" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -2168,15 +2203,15 @@
       </c>
       <c r="C5" s="27">
         <f t="shared" ref="C5:C7" ca="1" si="1">RANDBETWEEN(0,9)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -2185,15 +2220,15 @@
       </c>
       <c r="C6" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
@@ -2202,24 +2237,24 @@
       </c>
       <c r="C7" s="29">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D7" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E7" s="30">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="25"/>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="58" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="49"/>
-      <c r="E8" s="50"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="60"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="27"/>
@@ -2239,15 +2274,15 @@
       </c>
       <c r="C10" s="25">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D10" s="47">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E10" s="26">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -2256,15 +2291,15 @@
       </c>
       <c r="C11" s="27">
         <f t="shared" ref="C11:C13" ca="1" si="2">RANDBETWEEN(0,9)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D11" s="43">
         <f t="shared" ref="D11:E13" ca="1" si="3">RANDBETWEEN(0,9)</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E11" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
@@ -2273,7 +2308,7 @@
       </c>
       <c r="C12" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D12" s="43">
         <f t="shared" ca="1" si="3"/>
@@ -2281,7 +2316,7 @@
       </c>
       <c r="E12" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -2290,24 +2325,24 @@
       </c>
       <c r="C13" s="29">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D13" s="42">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E13" s="30">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="25"/>
-      <c r="C14" s="48" t="s">
+      <c r="C14" s="58" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="49"/>
-      <c r="E14" s="50"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="60"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="27"/>
@@ -2327,15 +2362,15 @@
       </c>
       <c r="C16" s="25">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D16" s="47">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E16" s="26">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -2344,15 +2379,15 @@
       </c>
       <c r="C17" s="27">
         <f t="shared" ref="C17:C19" ca="1" si="4">RANDBETWEEN(0,9)</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D17" s="43">
         <f t="shared" ref="D17:E19" ca="1" si="5">RANDBETWEEN(0,9)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E17" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -2361,11 +2396,11 @@
       </c>
       <c r="C18" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D18" s="43">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E18" s="28">
         <f t="shared" ca="1" si="5"/>
@@ -2378,24 +2413,24 @@
       </c>
       <c r="C19" s="29">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D19" s="42">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E19" s="30">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="25"/>
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="58" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="49"/>
-      <c r="E20" s="50"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="60"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="27"/>
@@ -2415,15 +2450,15 @@
       </c>
       <c r="C22" s="25">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D22" s="47">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E22" s="26">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -2432,15 +2467,15 @@
       </c>
       <c r="C23" s="27">
         <f t="shared" ref="C23:E25" ca="1" si="6">RANDBETWEEN(0,9)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D23" s="43">
         <f t="shared" ca="1" si="6"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E23" s="28">
         <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -2449,7 +2484,7 @@
       </c>
       <c r="C24" s="27">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D24" s="43">
         <f t="shared" ca="1" si="6"/>
@@ -2457,7 +2492,7 @@
       </c>
       <c r="E24" s="28">
         <f t="shared" ca="1" si="6"/>
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
@@ -2466,15 +2501,15 @@
       </c>
       <c r="C25" s="29">
         <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D25" s="42">
         <f t="shared" ca="1" si="6"/>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E25" s="30">
         <f t="shared" ca="1" si="6"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2860,12 +2895,12 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="49" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="53" t="s">
+      <c r="A4" s="50" t="s">
         <v>45</v>
       </c>
     </row>
@@ -2875,12 +2910,12 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="51" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="55" t="s">
+      <c r="A7" s="52" t="s">
         <v>49</v>
       </c>
     </row>
@@ -2895,12 +2930,12 @@
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="56" t="s">
+      <c r="A10" s="53" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="54" t="s">
         <v>52</v>
       </c>
     </row>
@@ -2915,7 +2950,7 @@
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="58" t="s">
+      <c r="A14" s="55" t="s">
         <v>55</v>
       </c>
     </row>
@@ -3030,9 +3065,47 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="62" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="61" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3043,10 +3116,10 @@
       <c r="A1" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="60">
+      <c r="B1" s="57">
         <v>43101</v>
       </c>
-      <c r="C1" s="60">
+      <c r="C1" s="57">
         <v>42736</v>
       </c>
     </row>
@@ -3378,7 +3451,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="56" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -3392,7 +3465,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="59" t="s">
+      <c r="A2" s="56" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="7">

</xml_diff>

<commit_message>
Add comments to worked-examples vignette
</commit_message>
<xml_diff>
--- a/inst/extdata/worked-examples.xlsx
+++ b/inst/extdata/worked-examples.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="13785" windowHeight="12660" firstSheet="12" activeTab="20"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="13785" windowHeight="12660" firstSheet="12" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="clean" sheetId="17" r:id="rId1"/>
@@ -29,13 +29,50 @@
     <sheet name="in-cell formatting" sheetId="19" r:id="rId20"/>
     <sheet name="superscript symbols" sheetId="22" r:id="rId21"/>
     <sheet name="non-text headers" sheetId="21" r:id="rId22"/>
+    <sheet name="comments" sheetId="23" r:id="rId23"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>nacnudus</author>
+  </authors>
+  <commentList>
+    <comment ref="A2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Absent Term 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Predicted</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="64">
   <si>
     <t>Title text</t>
   </si>
@@ -355,7 +392,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="30" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -573,6 +610,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="35">
@@ -1821,11 +1864,11 @@
       </c>
       <c r="D3" s="43">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3" s="43">
         <f t="shared" ref="E3:F18" ca="1" si="0">RANDBETWEEN(0,9)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F3" s="28">
         <f t="shared" ca="1" si="0"/>
@@ -1839,15 +1882,15 @@
       </c>
       <c r="D4" s="43">
         <f t="shared" ref="D4:D6" ca="1" si="1">RANDBETWEEN(0,9)</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E4" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -1857,7 +1900,7 @@
       </c>
       <c r="D5" s="43">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E5" s="43">
         <f t="shared" ca="1" si="0"/>
@@ -1865,7 +1908,7 @@
       </c>
       <c r="F5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -1875,15 +1918,15 @@
       </c>
       <c r="D6" s="43">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E6" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -1908,15 +1951,15 @@
       </c>
       <c r="D8" s="43">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E8" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -1926,15 +1969,15 @@
       </c>
       <c r="D9" s="43">
         <f t="shared" ref="D9:D11" ca="1" si="2">RANDBETWEEN(0,9)</f>
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E9" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -1944,15 +1987,15 @@
       </c>
       <c r="D10" s="43">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E10" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="F10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -1962,15 +2005,15 @@
       </c>
       <c r="D11" s="43">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E11" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F11" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -1995,15 +2038,15 @@
       </c>
       <c r="D13" s="43">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E13" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F13" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -2013,15 +2056,15 @@
       </c>
       <c r="D14" s="43">
         <f t="shared" ref="D14:D16" ca="1" si="3">RANDBETWEEN(0,9)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E14" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="F14" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -2031,15 +2074,15 @@
       </c>
       <c r="D15" s="43">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E15" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
@@ -2049,15 +2092,15 @@
       </c>
       <c r="D16" s="43">
         <f t="shared" ca="1" si="3"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="E16" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F16" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -2086,11 +2129,11 @@
       </c>
       <c r="E18" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
@@ -2100,15 +2143,15 @@
       </c>
       <c r="D19" s="43">
         <f t="shared" ref="D19:F21" ca="1" si="4">RANDBETWEEN(0,9)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E19" s="43">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F19" s="28">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -2118,7 +2161,7 @@
       </c>
       <c r="D20" s="43">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E20" s="43">
         <f t="shared" ca="1" si="4"/>
@@ -2136,15 +2179,15 @@
       </c>
       <c r="D21" s="42">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E21" s="42">
         <f t="shared" ca="1" si="4"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="F21" s="30">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2186,15 +2229,15 @@
       </c>
       <c r="C4" s="25">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D4" s="47">
         <f t="shared" ref="D4:E7" ca="1" si="0">RANDBETWEEN(0,9)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E4" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -2203,7 +2246,7 @@
       </c>
       <c r="C5" s="27">
         <f t="shared" ref="C5:C7" ca="1" si="1">RANDBETWEEN(0,9)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D5" s="43">
         <f t="shared" ca="1" si="0"/>
@@ -2211,7 +2254,7 @@
       </c>
       <c r="E5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -2220,15 +2263,15 @@
       </c>
       <c r="C6" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D6" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
@@ -2237,15 +2280,15 @@
       </c>
       <c r="C7" s="29">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D7" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E7" s="30">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
@@ -2274,15 +2317,15 @@
       </c>
       <c r="C10" s="25">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="D10" s="47">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E10" s="26">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -2291,11 +2334,11 @@
       </c>
       <c r="C11" s="27">
         <f t="shared" ref="C11:C13" ca="1" si="2">RANDBETWEEN(0,9)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D11" s="43">
         <f t="shared" ref="D11:E13" ca="1" si="3">RANDBETWEEN(0,9)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E11" s="28">
         <f t="shared" ca="1" si="3"/>
@@ -2308,15 +2351,15 @@
       </c>
       <c r="C12" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D12" s="43">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E12" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -2329,11 +2372,11 @@
       </c>
       <c r="D13" s="42">
         <f t="shared" ca="1" si="3"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E13" s="30">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -2362,15 +2405,15 @@
       </c>
       <c r="C16" s="25">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D16" s="47">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E16" s="26">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -2383,11 +2426,11 @@
       </c>
       <c r="D17" s="43">
         <f t="shared" ref="D17:E19" ca="1" si="5">RANDBETWEEN(0,9)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E17" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -2396,15 +2439,15 @@
       </c>
       <c r="C18" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="D18" s="43">
         <f t="shared" ca="1" si="5"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E18" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -2413,15 +2456,15 @@
       </c>
       <c r="C19" s="29">
         <f t="shared" ca="1" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D19" s="42">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E19" s="30">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -2450,15 +2493,15 @@
       </c>
       <c r="C22" s="25">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D22" s="47">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="26">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -2467,15 +2510,15 @@
       </c>
       <c r="C23" s="27">
         <f t="shared" ref="C23:E25" ca="1" si="6">RANDBETWEEN(0,9)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="D23" s="43">
         <f t="shared" ca="1" si="6"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E23" s="28">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
@@ -2484,15 +2527,15 @@
       </c>
       <c r="C24" s="27">
         <f t="shared" ca="1" si="6"/>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D24" s="43">
         <f t="shared" ca="1" si="6"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E24" s="28">
         <f t="shared" ca="1" si="6"/>
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
@@ -2501,15 +2544,15 @@
       </c>
       <c r="C25" s="29">
         <f t="shared" ca="1" si="6"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D25" s="42">
         <f t="shared" ca="1" si="6"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E25" s="30">
         <f t="shared" ca="1" si="6"/>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -3067,7 +3110,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3150,6 +3195,44 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="62" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="61">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="24">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>

</xml_diff>

<commit_message>
Vignette worked-example of ABOVE(), LEFT(), etc.
For centre-aligned headers
</commit_message>
<xml_diff>
--- a/inst/extdata/worked-examples.xlsx
+++ b/inst/extdata/worked-examples.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="13785" windowHeight="12660" firstSheet="12" activeTab="22"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="13785" windowHeight="12660" firstSheet="6" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="clean" sheetId="17" r:id="rId1"/>
@@ -16,20 +16,21 @@
     <sheet name="sentinels" sheetId="6" r:id="rId7"/>
     <sheet name="transposed" sheetId="20" r:id="rId8"/>
     <sheet name="pivot-annotations" sheetId="7" r:id="rId9"/>
-    <sheet name="pivot-notes" sheetId="9" r:id="rId10"/>
-    <sheet name="pivot-hierarchy" sheetId="10" r:id="rId11"/>
-    <sheet name="pivot-repeated-headers" sheetId="11" r:id="rId12"/>
-    <sheet name="pivot-header-within-data" sheetId="12" r:id="rId13"/>
-    <sheet name="small-multiples" sheetId="8" r:id="rId14"/>
-    <sheet name="humanities" sheetId="13" r:id="rId15"/>
-    <sheet name="performance" sheetId="14" r:id="rId16"/>
-    <sheet name="female" sheetId="15" r:id="rId17"/>
-    <sheet name="male" sheetId="16" r:id="rId18"/>
-    <sheet name="formatting" sheetId="18" r:id="rId19"/>
-    <sheet name="in-cell formatting" sheetId="19" r:id="rId20"/>
-    <sheet name="superscript symbols" sheetId="22" r:id="rId21"/>
-    <sheet name="non-text headers" sheetId="21" r:id="rId22"/>
-    <sheet name="comments" sheetId="23" r:id="rId23"/>
+    <sheet name="pivot-centre-aligned" sheetId="24" r:id="rId10"/>
+    <sheet name="pivot-notes" sheetId="9" r:id="rId11"/>
+    <sheet name="pivot-hierarchy" sheetId="10" r:id="rId12"/>
+    <sheet name="pivot-repeated-headers" sheetId="11" r:id="rId13"/>
+    <sheet name="pivot-header-within-data" sheetId="12" r:id="rId14"/>
+    <sheet name="small-multiples" sheetId="8" r:id="rId15"/>
+    <sheet name="humanities" sheetId="13" r:id="rId16"/>
+    <sheet name="performance" sheetId="14" r:id="rId17"/>
+    <sheet name="female" sheetId="15" r:id="rId18"/>
+    <sheet name="male" sheetId="16" r:id="rId19"/>
+    <sheet name="formatting" sheetId="18" r:id="rId20"/>
+    <sheet name="in-cell formatting" sheetId="19" r:id="rId21"/>
+    <sheet name="superscript symbols" sheetId="22" r:id="rId22"/>
+    <sheet name="non-text headers" sheetId="21" r:id="rId23"/>
+    <sheet name="comments" sheetId="23" r:id="rId24"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -72,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="71">
   <si>
     <t>Title text</t>
   </si>
@@ -386,6 +387,27 @@
       </rPr>
       <t>1</t>
     </r>
+  </si>
+  <si>
+    <t>Leah</t>
+  </si>
+  <si>
+    <t>Lenny</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Literature</t>
+  </si>
+  <si>
+    <t>Philosophy</t>
+  </si>
+  <si>
+    <t>Languages</t>
+  </si>
+  <si>
+    <t>Dance</t>
   </si>
 </sst>
 </file>
@@ -1154,7 +1176,7 @@
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1217,6 +1239,11 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="7" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1226,8 +1253,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1621,6 +1646,279 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:J11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="24"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D2" s="25"/>
+      <c r="E2" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="26"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="26"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="D3" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="61" t="s">
+        <v>66</v>
+      </c>
+      <c r="I3" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="25"/>
+      <c r="C4" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="25">
+        <v>3</v>
+      </c>
+      <c r="E4" s="62">
+        <v>1</v>
+      </c>
+      <c r="F4" s="20">
+        <v>2</v>
+      </c>
+      <c r="G4" s="21">
+        <v>4</v>
+      </c>
+      <c r="H4" s="62">
+        <v>3</v>
+      </c>
+      <c r="I4" s="62">
+        <v>3</v>
+      </c>
+      <c r="J4" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="27" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="27">
+        <v>8</v>
+      </c>
+      <c r="E5" s="60">
+        <v>3</v>
+      </c>
+      <c r="F5" s="18">
+        <v>4</v>
+      </c>
+      <c r="G5" s="19">
+        <v>7</v>
+      </c>
+      <c r="H5" s="60">
+        <v>5</v>
+      </c>
+      <c r="I5" s="60">
+        <v>5</v>
+      </c>
+      <c r="J5" s="28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="27"/>
+      <c r="C6" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="27">
+        <v>1</v>
+      </c>
+      <c r="E6" s="43">
+        <v>1</v>
+      </c>
+      <c r="F6" s="28">
+        <v>9</v>
+      </c>
+      <c r="G6" s="27">
+        <v>3</v>
+      </c>
+      <c r="H6" s="43">
+        <v>12</v>
+      </c>
+      <c r="I6" s="43">
+        <v>7</v>
+      </c>
+      <c r="J6" s="28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="27"/>
+      <c r="C7" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="27">
+        <v>5</v>
+      </c>
+      <c r="E7" s="43">
+        <v>10</v>
+      </c>
+      <c r="F7" s="28">
+        <v>10</v>
+      </c>
+      <c r="G7" s="27">
+        <v>8</v>
+      </c>
+      <c r="H7" s="43">
+        <v>2</v>
+      </c>
+      <c r="I7" s="43">
+        <v>5</v>
+      </c>
+      <c r="J7" s="28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="29"/>
+      <c r="C8" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" s="29">
+        <v>5</v>
+      </c>
+      <c r="E8" s="42">
+        <v>4</v>
+      </c>
+      <c r="F8" s="30">
+        <v>5</v>
+      </c>
+      <c r="G8" s="29">
+        <v>9</v>
+      </c>
+      <c r="H8" s="42">
+        <v>8</v>
+      </c>
+      <c r="I8" s="42">
+        <v>3</v>
+      </c>
+      <c r="J8" s="30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="25"/>
+      <c r="C9" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="25">
+        <v>4</v>
+      </c>
+      <c r="E9" s="47">
+        <v>10</v>
+      </c>
+      <c r="F9" s="26">
+        <v>10</v>
+      </c>
+      <c r="G9" s="25">
+        <v>2</v>
+      </c>
+      <c r="H9" s="47">
+        <v>4</v>
+      </c>
+      <c r="I9" s="47">
+        <v>5</v>
+      </c>
+      <c r="J9" s="26">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="27">
+        <v>4</v>
+      </c>
+      <c r="E10" s="60">
+        <v>5</v>
+      </c>
+      <c r="F10" s="18">
+        <v>6</v>
+      </c>
+      <c r="G10" s="19">
+        <v>4</v>
+      </c>
+      <c r="H10" s="60">
+        <v>12</v>
+      </c>
+      <c r="I10" s="60">
+        <v>9</v>
+      </c>
+      <c r="J10" s="28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="29"/>
+      <c r="C11" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="29">
+        <v>2</v>
+      </c>
+      <c r="E11" s="61">
+        <v>7</v>
+      </c>
+      <c r="F11" s="23">
+        <v>8</v>
+      </c>
+      <c r="G11" s="16">
+        <v>6</v>
+      </c>
+      <c r="H11" s="61">
+        <v>1</v>
+      </c>
+      <c r="I11" s="61">
+        <v>12</v>
+      </c>
+      <c r="J11" s="30">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1743,7 +2041,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:E8"/>
   <sheetViews>
@@ -1834,7 +2132,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F21"/>
   <sheetViews>
@@ -1864,15 +2162,15 @@
       </c>
       <c r="D3" s="43">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E3" s="43">
         <f t="shared" ref="E3:F18" ca="1" si="0">RANDBETWEEN(0,9)</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="F3" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
@@ -1882,15 +2180,15 @@
       </c>
       <c r="D4" s="43">
         <f t="shared" ref="D4:D6" ca="1" si="1">RANDBETWEEN(0,9)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E4" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F4" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
@@ -1900,15 +2198,15 @@
       </c>
       <c r="D5" s="43">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
@@ -1918,15 +2216,15 @@
       </c>
       <c r="D6" s="43">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E6" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
@@ -1951,15 +2249,15 @@
       </c>
       <c r="D8" s="43">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E8" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F8" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -1969,7 +2267,7 @@
       </c>
       <c r="D9" s="43">
         <f t="shared" ref="D9:D11" ca="1" si="2">RANDBETWEEN(0,9)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E9" s="43">
         <f t="shared" ca="1" si="0"/>
@@ -1977,7 +2275,7 @@
       </c>
       <c r="F9" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -1987,15 +2285,15 @@
       </c>
       <c r="D10" s="43">
         <f t="shared" ca="1" si="2"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E10" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F10" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -2005,15 +2303,15 @@
       </c>
       <c r="D11" s="43">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E11" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F11" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -2038,15 +2336,15 @@
       </c>
       <c r="D13" s="43">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E13" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F13" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -2056,15 +2354,15 @@
       </c>
       <c r="D14" s="43">
         <f t="shared" ref="D14:D16" ca="1" si="3">RANDBETWEEN(0,9)</f>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E14" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="F14" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -2074,15 +2372,15 @@
       </c>
       <c r="D15" s="43">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E15" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
@@ -2092,15 +2390,15 @@
       </c>
       <c r="D16" s="43">
         <f t="shared" ca="1" si="3"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E16" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F16" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
@@ -2125,11 +2423,11 @@
       </c>
       <c r="D18" s="43">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18" s="28">
         <f t="shared" ca="1" si="0"/>
@@ -2143,15 +2441,15 @@
       </c>
       <c r="D19" s="43">
         <f t="shared" ref="D19:F21" ca="1" si="4">RANDBETWEEN(0,9)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E19" s="43">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F19" s="28">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
@@ -2161,15 +2459,15 @@
       </c>
       <c r="D20" s="43">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E20" s="43">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F20" s="28">
         <f t="shared" ca="1" si="4"/>
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
@@ -2179,11 +2477,11 @@
       </c>
       <c r="D21" s="42">
         <f t="shared" ca="1" si="4"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E21" s="42">
         <f t="shared" ca="1" si="4"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F21" s="30">
         <f t="shared" ca="1" si="4"/>
@@ -2195,7 +2493,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E25"/>
   <sheetViews>
@@ -2205,11 +2503,11 @@
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="25"/>
-      <c r="C2" s="58" t="s">
+      <c r="C2" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="59"/>
-      <c r="E2" s="60"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="65"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="27"/>
@@ -2229,15 +2527,15 @@
       </c>
       <c r="C4" s="25">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D4" s="47">
         <f t="shared" ref="D4:E7" ca="1" si="0">RANDBETWEEN(0,9)</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E4" s="26">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -2246,15 +2544,15 @@
       </c>
       <c r="C5" s="27">
         <f t="shared" ref="C5:C7" ca="1" si="1">RANDBETWEEN(0,9)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D5" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E5" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -2263,15 +2561,15 @@
       </c>
       <c r="C6" s="27">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D6" s="43">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="28">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
@@ -2280,24 +2578,24 @@
       </c>
       <c r="C7" s="29">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D7" s="42">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E7" s="30">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="25"/>
-      <c r="C8" s="58" t="s">
+      <c r="C8" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="D8" s="59"/>
-      <c r="E8" s="60"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="65"/>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="27"/>
@@ -2317,7 +2615,7 @@
       </c>
       <c r="C10" s="25">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D10" s="47">
         <f ca="1">RANDBETWEEN(0,9)</f>
@@ -2325,7 +2623,7 @@
       </c>
       <c r="E10" s="26">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -2334,15 +2632,15 @@
       </c>
       <c r="C11" s="27">
         <f t="shared" ref="C11:C13" ca="1" si="2">RANDBETWEEN(0,9)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D11" s="43">
         <f t="shared" ref="D11:E13" ca="1" si="3">RANDBETWEEN(0,9)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E11" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
@@ -2351,15 +2649,15 @@
       </c>
       <c r="C12" s="27">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D12" s="43">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E12" s="28">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -2368,7 +2666,7 @@
       </c>
       <c r="C13" s="29">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D13" s="42">
         <f t="shared" ca="1" si="3"/>
@@ -2376,16 +2674,16 @@
       </c>
       <c r="E13" s="30">
         <f t="shared" ca="1" si="3"/>
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" s="25"/>
-      <c r="C14" s="58" t="s">
+      <c r="C14" s="63" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="59"/>
-      <c r="E14" s="60"/>
+      <c r="D14" s="64"/>
+      <c r="E14" s="65"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" s="27"/>
@@ -2405,15 +2703,15 @@
       </c>
       <c r="C16" s="25">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="D16" s="47">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E16" s="26">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -2422,15 +2720,15 @@
       </c>
       <c r="C17" s="27">
         <f t="shared" ref="C17:C19" ca="1" si="4">RANDBETWEEN(0,9)</f>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D17" s="43">
         <f t="shared" ref="D17:E19" ca="1" si="5">RANDBETWEEN(0,9)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E17" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -2439,15 +2737,15 @@
       </c>
       <c r="C18" s="27">
         <f t="shared" ca="1" si="4"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D18" s="43">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E18" s="28">
         <f t="shared" ca="1" si="5"/>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -2456,7 +2754,7 @@
       </c>
       <c r="C19" s="29">
         <f t="shared" ca="1" si="4"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D19" s="42">
         <f t="shared" ca="1" si="5"/>
@@ -2464,16 +2762,16 @@
       </c>
       <c r="E19" s="30">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B20" s="25"/>
-      <c r="C20" s="58" t="s">
+      <c r="C20" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="D20" s="59"/>
-      <c r="E20" s="60"/>
+      <c r="D20" s="64"/>
+      <c r="E20" s="65"/>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B21" s="27"/>
@@ -2493,15 +2791,15 @@
       </c>
       <c r="C22" s="25">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D22" s="47">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E22" s="26">
         <f ca="1">RANDBETWEEN(0,9)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -2510,11 +2808,11 @@
       </c>
       <c r="C23" s="27">
         <f t="shared" ref="C23:E25" ca="1" si="6">RANDBETWEEN(0,9)</f>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D23" s="43">
         <f t="shared" ca="1" si="6"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="E23" s="28">
         <f t="shared" ca="1" si="6"/>
@@ -2527,15 +2825,15 @@
       </c>
       <c r="C24" s="27">
         <f t="shared" ca="1" si="6"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D24" s="43">
         <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E24" s="28">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.25">
@@ -2544,15 +2842,15 @@
       </c>
       <c r="C25" s="29">
         <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D25" s="42">
         <f t="shared" ca="1" si="6"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E25" s="30">
         <f t="shared" ca="1" si="6"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2567,7 +2865,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
@@ -2712,50 +3010,6 @@
       </c>
       <c r="G9" s="24" t="s">
         <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="30"/>
-      <c r="B1" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="42" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="43">
-        <v>1</v>
-      </c>
-      <c r="C2" s="43">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="43">
-        <v>3</v>
-      </c>
-      <c r="C3" s="43">
-        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2782,24 +3036,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="43">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2" s="43">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3" s="43">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C3" s="43">
-        <v>12</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2808,6 +3062,50 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="30"/>
+      <c r="B1" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="43">
+        <v>5</v>
+      </c>
+      <c r="C2" s="43">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="43">
+        <v>7</v>
+      </c>
+      <c r="C3" s="43">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -2858,7 +3156,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
@@ -2914,7 +3212,55 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -3003,55 +3349,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D7" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -3106,7 +3404,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -3117,10 +3415,10 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="59" t="s">
         <v>26</v>
       </c>
     </row>
@@ -3128,7 +3426,7 @@
       <c r="A2" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="61" t="s">
+      <c r="B2" s="58" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3146,7 +3444,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -3195,19 +3493,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="59" t="s">
         <v>26</v>
       </c>
     </row>
@@ -3215,7 +3513,7 @@
       <c r="A2" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="61">
+      <c r="B2" s="58">
         <v>9</v>
       </c>
     </row>

</xml_diff>